<commit_message>
Moved C linear decrease from strategy.py to MABsolver.py
</commit_message>
<xml_diff>
--- a/evaluations_fixed_parameters/Results_fixed.xlsx
+++ b/evaluations_fixed_parameters/Results_fixed.xlsx
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AB17" sqref="V17:AB19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,24 +688,24 @@
       <c r="R3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S3" t="e">
-        <f>MATCH(MAX(S8:S29),S8:S11,0)</f>
-        <v>#N/A</v>
+      <c r="S3">
+        <f>MATCH(MAX(S8:S29),S8:S110,0)</f>
+        <v>5</v>
       </c>
       <c r="T3">
-        <f>MATCH(MIN(T8:T29),T8:T11,0)</f>
+        <f>MATCH(MIN(T8:T29),T8:T110,0)</f>
         <v>1</v>
       </c>
       <c r="U3">
-        <f>MATCH(MAX(U8:U29),U8:U11,0)</f>
+        <f>MATCH(MAX(U8:U29),U8:U110,0)</f>
         <v>1</v>
       </c>
-      <c r="V3" t="e">
-        <f t="shared" ref="V3:BG3" si="0">MATCH(MAX(V8:V29),V8:V11,0)</f>
-        <v>#N/A</v>
+      <c r="V3">
+        <f>MATCH(MAX(V8:V29),V8:V29,0)</f>
+        <v>5</v>
       </c>
       <c r="W3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="W3:BG3" si="0">MATCH(MAX(W8:W29),W8:W29,0)</f>
         <v>3</v>
       </c>
       <c r="X3" s="6">
@@ -716,13 +716,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="Z3" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA3" s="6" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="Z3" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AA3" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="AB3" s="6">
         <f t="shared" si="0"/>
@@ -760,21 +760,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AK3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="AK3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="AM3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AN3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="AN3">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="AO3">
         <f t="shared" si="0"/>
@@ -784,17 +784,17 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AQ3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AR3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AS3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="AQ3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AR3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AS3">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="AT3">
         <f t="shared" si="0"/>
@@ -828,13 +828,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="BB3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="BC3" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="BB3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="BC3">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="BD3">
         <f t="shared" si="0"/>
@@ -1862,6 +1862,9 @@
       </c>
     </row>
     <row r="12" spans="1:60" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
       <c r="B12" s="10" t="s">
         <v>73</v>
       </c>
@@ -1879,8 +1882,8 @@
         <v>49.33</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>COUNTIF(W$3:BG$3,CONCATENATE("=",TEXT($A12,"d")))</f>
+        <v>10</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="2"/>
@@ -1888,7 +1891,7 @@
       </c>
       <c r="L12" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12" s="7">
         <f t="shared" si="4"/>
@@ -1896,7 +1899,7 @@
       </c>
       <c r="N12" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O12" s="7">
         <f t="shared" si="6"/>
@@ -1904,7 +1907,7 @@
       </c>
       <c r="P12" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R12" s="12" t="s">
         <v>75</v>
@@ -2032,9 +2035,7 @@
       <c r="BG12" s="12">
         <v>23.33</v>
       </c>
-      <c r="BH12" s="12">
-        <v>71.23</v>
-      </c>
+      <c r="BH12" s="12"/>
     </row>
     <row r="13" spans="1:60" x14ac:dyDescent="0.25">
       <c r="M13" s="11"/>

</xml_diff>

<commit_message>
voter + HP results
</commit_message>
<xml_diff>
--- a/evaluations_fixed_parameters/Results_fixed.xlsx
+++ b/evaluations_fixed_parameters/Results_fixed.xlsx
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,15 +1224,15 @@
       </c>
       <c r="V3">
         <f>MATCH(MIN(V8:V126),V8:V126,0)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:BI3" si="0">MATCH(MAX(W8:W126),W8:W126,0)</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="X3" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="AE3" s="4">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AF3" s="4">
         <f t="shared" si="0"/>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="AO3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AP3">
         <f t="shared" si="0"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AY3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AZ3">
         <f t="shared" si="0"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="BB3">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="BC3">
         <f t="shared" si="0"/>
@@ -2988,7 +2988,7 @@
         <v>74</v>
       </c>
       <c r="J17" s="14">
-        <f t="shared" ref="J17" si="9">X17</f>
+        <f t="shared" ref="J17:J18" si="9">X17</f>
         <v>52.01</v>
       </c>
       <c r="K17" s="14">
@@ -3004,23 +3004,23 @@
         <v>52.346000000000004</v>
       </c>
       <c r="N17" s="19">
-        <f t="shared" ref="N17" si="10">(SUM(Y17:AC17))/(COUNT(Y17:AC17))</f>
+        <f t="shared" ref="N17:N18" si="10">(SUM(Y17:AC17))/(COUNT(Y17:AC17))</f>
         <v>53.179999999999993</v>
       </c>
       <c r="O17" s="19">
-        <f t="shared" ref="O17" si="11">(SUM(AD17:AH17))/(COUNT(AD17:AH17))</f>
+        <f t="shared" ref="O17:O18" si="11">(SUM(AD17:AH17))/(COUNT(AD17:AH17))</f>
         <v>51.512</v>
       </c>
       <c r="P17" s="14">
-        <f t="shared" ref="P17" si="12">AVERAGE(AI17:BI17)</f>
+        <f t="shared" ref="P17:P18" si="12">AVERAGE(AI17:BI17)</f>
         <v>51.880370370370379</v>
       </c>
       <c r="Q17" s="14">
-        <f t="shared" ref="Q17" si="13">(SUM(AI17:AU17))/(COUNT(AI17:AU17))</f>
+        <f t="shared" ref="Q17:Q18" si="13">(SUM(AI17:AU17))/(COUNT(AI17:AU17))</f>
         <v>55.869230769230768</v>
       </c>
       <c r="R17" s="14">
-        <f t="shared" ref="R17" si="14">(SUM(AV17:BI17))/(COUNT(AV17:BI17))</f>
+        <f t="shared" ref="R17:R18" si="14">(SUM(AV17:BI17))/(COUNT(AV17:BI17))</f>
         <v>48.176428571428566</v>
       </c>
       <c r="T17" s="25">
@@ -3166,58 +3166,169 @@
       <c r="F18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
+      <c r="J18" s="14">
+        <f t="shared" si="9"/>
+        <v>54.01</v>
+      </c>
+      <c r="K18" s="14">
+        <f>(SUM(Y18:AC18)+SUM(AI18:AU18))/(COUNT(Y18:AC18)+COUNT(AI18:AU18))</f>
+        <v>53.37722222222223</v>
+      </c>
+      <c r="L18" s="14">
+        <f>(SUM(AD18:AH18)+SUM(AV18:BI18))/(COUNT(AD18:AH18)+COUNT(AV18:BI18))</f>
+        <v>54.608947368421049</v>
+      </c>
+      <c r="M18" s="19">
+        <f>AVERAGE(Y18:AH18)</f>
+        <v>59.613999999999997</v>
+      </c>
+      <c r="N18" s="19">
+        <f t="shared" si="10"/>
+        <v>52.057999999999993</v>
+      </c>
+      <c r="O18" s="19">
+        <f t="shared" si="11"/>
+        <v>67.169999999999987</v>
+      </c>
+      <c r="P18" s="14">
+        <f t="shared" si="12"/>
+        <v>51.934074074074076</v>
+      </c>
+      <c r="Q18" s="14">
+        <f t="shared" si="13"/>
+        <v>53.884615384615394</v>
+      </c>
+      <c r="R18" s="14">
+        <f t="shared" si="14"/>
+        <v>50.122857142857143</v>
+      </c>
       <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
-      <c r="AD18" s="24"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="24"/>
-      <c r="AG18" s="24"/>
-      <c r="AH18" s="24"/>
-      <c r="AI18" s="22"/>
-      <c r="AJ18" s="22"/>
-      <c r="AK18" s="22"/>
-      <c r="AL18" s="22"/>
-      <c r="AM18" s="22"/>
-      <c r="AN18" s="22"/>
-      <c r="AO18" s="22"/>
-      <c r="AP18" s="22"/>
-      <c r="AQ18" s="22"/>
-      <c r="AR18" s="22"/>
-      <c r="AS18" s="22"/>
-      <c r="AT18" s="22"/>
-      <c r="AU18" s="22"/>
-      <c r="AV18" s="22"/>
-      <c r="AW18" s="22"/>
-      <c r="AX18" s="22"/>
-      <c r="AY18" s="22"/>
-      <c r="AZ18" s="22"/>
-      <c r="BA18" s="22"/>
-      <c r="BB18" s="22"/>
-      <c r="BC18" s="22"/>
-      <c r="BD18" s="22"/>
-      <c r="BE18" s="22"/>
-      <c r="BF18" s="22"/>
-      <c r="BG18" s="22"/>
-      <c r="BH18" s="22"/>
-      <c r="BI18" s="22"/>
+      <c r="T18">
+        <v>1000</v>
+      </c>
+      <c r="U18" s="2">
+        <v>52678.43</v>
+      </c>
+      <c r="V18" s="2">
+        <v>2174.0700000000002</v>
+      </c>
+      <c r="W18" s="2">
+        <v>91.84</v>
+      </c>
+      <c r="X18" s="23">
+        <v>54.01</v>
+      </c>
+      <c r="Y18" s="24">
+        <v>85.45</v>
+      </c>
+      <c r="Z18" s="24">
+        <v>68.62</v>
+      </c>
+      <c r="AA18" s="24">
+        <v>71.34</v>
+      </c>
+      <c r="AB18" s="24">
+        <v>25.51</v>
+      </c>
+      <c r="AC18" s="24">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="AD18" s="24">
+        <v>69.989999999999995</v>
+      </c>
+      <c r="AE18" s="24">
+        <v>59.37</v>
+      </c>
+      <c r="AF18" s="24">
+        <v>75.569999999999993</v>
+      </c>
+      <c r="AG18" s="24">
+        <v>82.34</v>
+      </c>
+      <c r="AH18" s="24">
+        <v>48.58</v>
+      </c>
+      <c r="AI18" s="22">
+        <v>97.31</v>
+      </c>
+      <c r="AJ18" s="22">
+        <v>91.32</v>
+      </c>
+      <c r="AK18" s="22">
+        <v>23.3</v>
+      </c>
+      <c r="AL18" s="22">
+        <v>99.15</v>
+      </c>
+      <c r="AM18" s="22">
+        <v>19.12</v>
+      </c>
+      <c r="AN18" s="22">
+        <v>13.17</v>
+      </c>
+      <c r="AO18" s="22">
+        <v>67.16</v>
+      </c>
+      <c r="AP18" s="22">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="AQ18" s="22">
+        <v>60.64</v>
+      </c>
+      <c r="AR18" s="22">
+        <v>15.5</v>
+      </c>
+      <c r="AS18" s="22">
+        <v>37.590000000000003</v>
+      </c>
+      <c r="AT18" s="22">
+        <v>75.52</v>
+      </c>
+      <c r="AU18" s="22">
+        <v>84.62</v>
+      </c>
+      <c r="AV18" s="22">
+        <v>13.39</v>
+      </c>
+      <c r="AW18" s="22">
+        <v>93.87</v>
+      </c>
+      <c r="AX18" s="22">
+        <v>39.549999999999997</v>
+      </c>
+      <c r="AY18" s="22">
+        <v>37.32</v>
+      </c>
+      <c r="AZ18" s="22">
+        <v>56.26</v>
+      </c>
+      <c r="BA18" s="22">
+        <v>41.42</v>
+      </c>
+      <c r="BB18" s="22">
+        <v>64.150000000000006</v>
+      </c>
+      <c r="BC18" s="22">
+        <v>63.27</v>
+      </c>
+      <c r="BD18" s="22">
+        <v>11.02</v>
+      </c>
+      <c r="BE18" s="22">
+        <v>25.26</v>
+      </c>
+      <c r="BF18" s="22">
+        <v>75.16</v>
+      </c>
+      <c r="BG18" s="22">
+        <v>71.48</v>
+      </c>
+      <c r="BH18" s="22">
+        <v>58.48</v>
+      </c>
+      <c r="BI18" s="22">
+        <v>51.09</v>
+      </c>
       <c r="BJ18" s="8"/>
       <c r="BL18"/>
     </row>

</xml_diff>

<commit_message>
Results sum of rewards
</commit_message>
<xml_diff>
--- a/evaluations_fixed_parameters/Results_fixed.xlsx
+++ b/evaluations_fixed_parameters/Results_fixed.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Summary (stddev)" sheetId="6" r:id="rId2"/>
-    <sheet name="UCBT_lin2C_6par" sheetId="3" r:id="rId3"/>
-    <sheet name="6par_calc" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="Summary (stddev)" sheetId="6" r:id="rId3"/>
+    <sheet name="UCBT_lin2C_6par" sheetId="3" r:id="rId4"/>
+    <sheet name="6par_calc" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="124">
   <si>
     <t>repeat</t>
   </si>
@@ -387,6 +388,9 @@
   <si>
     <t>UCBT_C=0.77</t>
   </si>
+  <si>
+    <t>FINAL EVAL: sum of rewards</t>
+  </si>
 </sst>
 </file>
 
@@ -655,7 +659,742 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="344">
+  <dxfs count="449">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3366,8 +4105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3417,7 +4156,7 @@
       </c>
       <c r="V3">
         <f>MATCH(MIN(V8:V134),V8:V134,0)</f>
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:BI3" si="0">MATCH(MAX(W8:W134),W8:W134,0)</f>
@@ -3425,47 +4164,47 @@
       </c>
       <c r="X3" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="Z3" s="4">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="AA3" s="4">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="AB3" s="4">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="AC3" s="4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="AD3" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="AE3" s="4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="AF3" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="AH3" s="4">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="AI3">
         <f t="shared" si="0"/>
@@ -7328,7 +8067,9 @@
         <v>49.156190476190474</v>
       </c>
       <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
+      <c r="T29" s="25">
+        <v>1000</v>
+      </c>
       <c r="U29" s="14">
         <v>52798.829999999994</v>
       </c>
@@ -11094,6 +11835,9 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
+      <c r="B54" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="J54" s="14"/>
       <c r="K54" s="14"/>
       <c r="L54" s="14"/>
@@ -11148,27 +11892,82 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
+      <c r="B55" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="6"/>
+      <c r="F55" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="J55" s="14"/>
       <c r="K55" s="14"/>
       <c r="L55" s="14"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
+      <c r="M55" s="19">
+        <f>AVERAGE(Y55:AH55)</f>
+        <v>350.9375</v>
+      </c>
+      <c r="N55" s="19">
+        <f>(SUM(Y55:AC55))/(COUNT(Y55:AC55))</f>
+        <v>217.34699999999998</v>
+      </c>
+      <c r="O55" s="19">
+        <f>(SUM(AD55:AH55))/(COUNT(AD55:AH55))</f>
+        <v>484.52800000000008</v>
+      </c>
       <c r="P55" s="14"/>
       <c r="Q55" s="14"/>
       <c r="R55" s="14"/>
-      <c r="U55" s="14"/>
-      <c r="X55" s="23"/>
-      <c r="Y55" s="19"/>
-      <c r="Z55" s="19"/>
-      <c r="AA55" s="19"/>
-      <c r="AB55" s="19"/>
-      <c r="AC55" s="19"/>
-      <c r="AD55" s="19"/>
-      <c r="AE55" s="19"/>
-      <c r="AF55" s="19"/>
-      <c r="AG55" s="19"/>
-      <c r="AH55" s="19"/>
+      <c r="T55">
+        <v>3118</v>
+      </c>
+      <c r="U55" s="14">
+        <v>3509.375</v>
+      </c>
+      <c r="V55" s="2">
+        <v>409.625</v>
+      </c>
+      <c r="W55" s="2">
+        <v>90.164999999999992</v>
+      </c>
+      <c r="X55" s="23">
+        <v>57.06</v>
+      </c>
+      <c r="Y55" s="19">
+        <v>292.70999999999998</v>
+      </c>
+      <c r="Z55" s="19">
+        <v>280.48500000000001</v>
+      </c>
+      <c r="AA55" s="19">
+        <v>185.94</v>
+      </c>
+      <c r="AB55" s="19">
+        <v>223.82</v>
+      </c>
+      <c r="AC55" s="19">
+        <v>103.78</v>
+      </c>
+      <c r="AD55" s="19">
+        <v>549.82749999999999</v>
+      </c>
+      <c r="AE55" s="19">
+        <v>452.09249999999997</v>
+      </c>
+      <c r="AF55" s="19">
+        <v>573.8325000000001</v>
+      </c>
+      <c r="AG55" s="19">
+        <v>375.9375</v>
+      </c>
+      <c r="AH55" s="19">
+        <v>470.95000000000005</v>
+      </c>
       <c r="AI55" s="31"/>
       <c r="AJ55" s="31"/>
       <c r="AK55" s="31"/>
@@ -11201,6 +12000,19 @@
       <c r="A56" s="50">
         <f t="shared" si="1"/>
         <v>49</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="F56" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="U56" s="12"/>
       <c r="Y56" s="17"/>
@@ -12166,292 +12978,292 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Y91:Y100">
-    <cfRule type="top10" priority="252" rank="20"/>
+    <cfRule type="top10" priority="255" rank="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J72:J90">
-    <cfRule type="top10" dxfId="343" priority="160" rank="2"/>
+    <cfRule type="top10" dxfId="293" priority="163" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72:K90">
-    <cfRule type="top10" dxfId="342" priority="159" rank="2"/>
+    <cfRule type="top10" dxfId="292" priority="162" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L72:L90">
-    <cfRule type="top10" dxfId="341" priority="158" rank="2"/>
+    <cfRule type="top10" dxfId="291" priority="161" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M72:M90">
-    <cfRule type="top10" dxfId="340" priority="157" rank="2"/>
+    <cfRule type="top10" dxfId="290" priority="160" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N72:N90">
-    <cfRule type="top10" dxfId="339" priority="156" rank="2"/>
+    <cfRule type="top10" dxfId="289" priority="159" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O72:O90">
-    <cfRule type="top10" dxfId="338" priority="155" rank="2"/>
+    <cfRule type="top10" dxfId="288" priority="158" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P72:P90">
-    <cfRule type="top10" dxfId="337" priority="154" rank="2"/>
+    <cfRule type="top10" dxfId="287" priority="157" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q72:Q90">
-    <cfRule type="top10" dxfId="336" priority="153" rank="2"/>
+    <cfRule type="top10" dxfId="286" priority="156" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R72:R90">
-    <cfRule type="top10" dxfId="335" priority="152" rank="2"/>
+    <cfRule type="top10" dxfId="285" priority="155" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y72:Y90">
-    <cfRule type="top10" dxfId="334" priority="151" rank="2"/>
+    <cfRule type="top10" dxfId="284" priority="154" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X66:X90">
-    <cfRule type="top10" dxfId="333" priority="150" rank="2"/>
+    <cfRule type="top10" dxfId="283" priority="153" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z72:Z82">
-    <cfRule type="top10" dxfId="332" priority="149" rank="2"/>
+    <cfRule type="top10" dxfId="282" priority="152" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA72:AA82">
-    <cfRule type="top10" dxfId="331" priority="148" rank="2"/>
+    <cfRule type="top10" dxfId="281" priority="151" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB72:AB82">
-    <cfRule type="top10" dxfId="330" priority="147" rank="2"/>
+    <cfRule type="top10" dxfId="280" priority="150" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC72:AC82">
-    <cfRule type="top10" dxfId="329" priority="146" rank="2"/>
+    <cfRule type="top10" dxfId="279" priority="149" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD72:AD82">
-    <cfRule type="top10" dxfId="328" priority="145" rank="2"/>
+    <cfRule type="top10" dxfId="278" priority="148" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE72:AE82">
-    <cfRule type="top10" dxfId="327" priority="144" rank="2"/>
+    <cfRule type="top10" dxfId="277" priority="147" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF72:AF82">
-    <cfRule type="top10" dxfId="326" priority="143" rank="2"/>
+    <cfRule type="top10" dxfId="276" priority="146" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG72:AG82">
-    <cfRule type="top10" dxfId="325" priority="142" rank="2"/>
+    <cfRule type="top10" dxfId="275" priority="145" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH72:AH82">
-    <cfRule type="top10" dxfId="324" priority="141" rank="2"/>
+    <cfRule type="top10" dxfId="274" priority="144" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI72:AI82">
-    <cfRule type="top10" dxfId="323" priority="140" rank="2"/>
+    <cfRule type="top10" dxfId="273" priority="143" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ72:AJ82">
-    <cfRule type="top10" dxfId="322" priority="139" rank="2"/>
+    <cfRule type="top10" dxfId="272" priority="142" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK72:AK82">
-    <cfRule type="top10" dxfId="321" priority="138" rank="2"/>
+    <cfRule type="top10" dxfId="271" priority="141" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL72:AL82">
-    <cfRule type="top10" dxfId="320" priority="137" rank="2"/>
+    <cfRule type="top10" dxfId="270" priority="140" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM72:AM82">
-    <cfRule type="top10" dxfId="319" priority="136" rank="2"/>
+    <cfRule type="top10" dxfId="269" priority="139" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN72:AN82">
-    <cfRule type="top10" dxfId="318" priority="135" rank="2"/>
+    <cfRule type="top10" dxfId="268" priority="138" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO72:AO82">
-    <cfRule type="top10" dxfId="317" priority="134" rank="2"/>
+    <cfRule type="top10" dxfId="267" priority="137" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP72:AP82">
-    <cfRule type="top10" dxfId="316" priority="133" rank="2"/>
+    <cfRule type="top10" dxfId="266" priority="136" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ72:AQ82">
-    <cfRule type="top10" dxfId="315" priority="132" rank="2"/>
+    <cfRule type="top10" dxfId="265" priority="135" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR72:AR82">
-    <cfRule type="top10" dxfId="314" priority="131" rank="2"/>
+    <cfRule type="top10" dxfId="264" priority="134" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS72:AS82">
-    <cfRule type="top10" dxfId="313" priority="130" rank="2"/>
+    <cfRule type="top10" dxfId="263" priority="133" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT72:AT82">
-    <cfRule type="top10" dxfId="312" priority="129" rank="2"/>
+    <cfRule type="top10" dxfId="262" priority="132" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU72:AU82">
-    <cfRule type="top10" dxfId="311" priority="128" rank="2"/>
+    <cfRule type="top10" dxfId="261" priority="131" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV72:AV82">
-    <cfRule type="top10" dxfId="310" priority="127" rank="2"/>
+    <cfRule type="top10" dxfId="260" priority="130" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW72:AW82">
-    <cfRule type="top10" dxfId="309" priority="126" rank="2"/>
+    <cfRule type="top10" dxfId="259" priority="129" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX72:AX82">
-    <cfRule type="top10" dxfId="308" priority="125" rank="2"/>
+    <cfRule type="top10" dxfId="258" priority="128" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY72:AY82">
-    <cfRule type="top10" dxfId="307" priority="124" rank="2"/>
+    <cfRule type="top10" dxfId="257" priority="127" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ72:AZ82">
-    <cfRule type="top10" dxfId="306" priority="123" rank="2"/>
+    <cfRule type="top10" dxfId="256" priority="126" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA72:BA82">
-    <cfRule type="top10" dxfId="305" priority="122" rank="2"/>
+    <cfRule type="top10" dxfId="255" priority="125" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB72:BB82">
-    <cfRule type="top10" dxfId="304" priority="121" rank="2"/>
+    <cfRule type="top10" dxfId="254" priority="124" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC72:BC82">
-    <cfRule type="top10" dxfId="303" priority="120" rank="2"/>
+    <cfRule type="top10" dxfId="253" priority="123" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD72:BD82">
-    <cfRule type="top10" dxfId="302" priority="119" rank="2"/>
+    <cfRule type="top10" dxfId="252" priority="122" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE72:BE82">
-    <cfRule type="top10" dxfId="301" priority="118" rank="2"/>
+    <cfRule type="top10" dxfId="251" priority="121" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF72:BF82">
-    <cfRule type="top10" dxfId="300" priority="117" rank="2"/>
+    <cfRule type="top10" dxfId="250" priority="120" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG72:BG82">
-    <cfRule type="top10" dxfId="299" priority="116" rank="2"/>
+    <cfRule type="top10" dxfId="249" priority="119" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH72:BH82">
-    <cfRule type="top10" dxfId="298" priority="115" rank="2"/>
+    <cfRule type="top10" dxfId="248" priority="118" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI72:BI82">
-    <cfRule type="top10" dxfId="297" priority="114" rank="2"/>
+    <cfRule type="top10" dxfId="247" priority="117" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U72:U75">
-    <cfRule type="top10" dxfId="296" priority="113" rank="2"/>
+    <cfRule type="top10" dxfId="246" priority="116" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:J71">
-    <cfRule type="top10" dxfId="295" priority="672" rank="2"/>
+    <cfRule type="top10" dxfId="245" priority="675" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K71">
-    <cfRule type="top10" dxfId="294" priority="674" rank="2"/>
+    <cfRule type="top10" dxfId="244" priority="677" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L71">
-    <cfRule type="top10" dxfId="293" priority="676" rank="2"/>
+    <cfRule type="top10" dxfId="243" priority="679" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8:P71">
-    <cfRule type="top10" dxfId="292" priority="678" rank="2"/>
+    <cfRule type="top10" dxfId="242" priority="681" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Q71">
-    <cfRule type="top10" dxfId="291" priority="680" rank="2"/>
+    <cfRule type="top10" dxfId="241" priority="683" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:R71">
-    <cfRule type="top10" dxfId="290" priority="682" rank="2"/>
+    <cfRule type="top10" dxfId="240" priority="685" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U8:U71">
-    <cfRule type="top10" dxfId="289" priority="684" rank="2"/>
+  <conditionalFormatting sqref="U8:U54 U57:U71">
+    <cfRule type="top10" dxfId="239" priority="687" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8:M71">
-    <cfRule type="top10" dxfId="288" priority="686" rank="2"/>
+  <conditionalFormatting sqref="M8:M54 M57:M71">
+    <cfRule type="top10" dxfId="238" priority="689" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:N71">
-    <cfRule type="top10" dxfId="287" priority="688" rank="2"/>
+  <conditionalFormatting sqref="N8:N54 N57:N71">
+    <cfRule type="top10" dxfId="237" priority="691" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O71">
-    <cfRule type="top10" dxfId="286" priority="690" rank="2"/>
+  <conditionalFormatting sqref="O8:O54 O57:O71">
+    <cfRule type="top10" dxfId="236" priority="693" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y8:Y71">
-    <cfRule type="top10" dxfId="285" priority="692" rank="2"/>
+  <conditionalFormatting sqref="Y8:Y54 Y57:Y71">
+    <cfRule type="top10" dxfId="235" priority="695" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z8:Z71">
-    <cfRule type="top10" dxfId="284" priority="694" rank="2"/>
+  <conditionalFormatting sqref="Z8:Z54 Z57:Z71">
+    <cfRule type="top10" dxfId="234" priority="697" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA8:AA71">
-    <cfRule type="top10" dxfId="283" priority="696" rank="2"/>
+  <conditionalFormatting sqref="AA8:AA54 AA57:AA71">
+    <cfRule type="top10" dxfId="233" priority="699" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB8:AB71">
-    <cfRule type="top10" dxfId="282" priority="698" rank="2"/>
+  <conditionalFormatting sqref="AB8:AB54 AB57:AB71">
+    <cfRule type="top10" dxfId="232" priority="701" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC8:AC71">
-    <cfRule type="top10" dxfId="281" priority="700" rank="2"/>
+  <conditionalFormatting sqref="AC8:AC54 AC57:AC71">
+    <cfRule type="top10" dxfId="231" priority="703" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD8:AD71">
-    <cfRule type="top10" dxfId="280" priority="702" rank="2"/>
+  <conditionalFormatting sqref="AD8:AD54 AD57:AD71">
+    <cfRule type="top10" dxfId="230" priority="705" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE8:AE71">
-    <cfRule type="top10" dxfId="279" priority="704" rank="2"/>
+  <conditionalFormatting sqref="AE8:AE54 AE57:AE71">
+    <cfRule type="top10" dxfId="229" priority="707" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF8:AF71">
-    <cfRule type="top10" dxfId="278" priority="706" rank="2"/>
+  <conditionalFormatting sqref="AF8:AF54 AF57:AF71">
+    <cfRule type="top10" dxfId="228" priority="709" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG8:AG71">
-    <cfRule type="top10" dxfId="277" priority="708" rank="2"/>
+  <conditionalFormatting sqref="AG8:AG54 AG57:AG71">
+    <cfRule type="top10" dxfId="227" priority="711" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH8:AH71">
-    <cfRule type="top10" dxfId="276" priority="710" rank="2"/>
+  <conditionalFormatting sqref="AH8:AH54 AH57:AH71">
+    <cfRule type="top10" dxfId="226" priority="713" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8:AI71">
-    <cfRule type="top10" dxfId="275" priority="712" rank="2"/>
+    <cfRule type="top10" dxfId="225" priority="715" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ71">
-    <cfRule type="top10" dxfId="274" priority="714" rank="2"/>
+    <cfRule type="top10" dxfId="224" priority="717" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8:AK71">
-    <cfRule type="top10" dxfId="273" priority="716" rank="2"/>
+    <cfRule type="top10" dxfId="223" priority="719" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL8:AL71">
-    <cfRule type="top10" dxfId="272" priority="718" rank="2"/>
+    <cfRule type="top10" dxfId="222" priority="721" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM8:AM71">
-    <cfRule type="top10" dxfId="271" priority="720" rank="2"/>
+    <cfRule type="top10" dxfId="221" priority="723" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN8:AN71">
-    <cfRule type="top10" dxfId="270" priority="722" rank="2"/>
+    <cfRule type="top10" dxfId="220" priority="725" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO8:AO71">
-    <cfRule type="top10" dxfId="269" priority="724" rank="2"/>
+    <cfRule type="top10" dxfId="219" priority="727" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP8:AP71">
-    <cfRule type="top10" dxfId="268" priority="726" rank="2"/>
+    <cfRule type="top10" dxfId="218" priority="729" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ8:AQ71">
-    <cfRule type="top10" dxfId="267" priority="728" rank="2"/>
+    <cfRule type="top10" dxfId="217" priority="731" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR8:AR71">
-    <cfRule type="top10" dxfId="266" priority="730" rank="2"/>
+    <cfRule type="top10" dxfId="216" priority="733" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS8:AS71">
-    <cfRule type="top10" dxfId="265" priority="732" rank="2"/>
+    <cfRule type="top10" dxfId="215" priority="735" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT8:AT71">
-    <cfRule type="top10" dxfId="264" priority="734" rank="2"/>
+    <cfRule type="top10" dxfId="214" priority="737" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU8:AU71">
-    <cfRule type="top10" dxfId="263" priority="736" rank="2"/>
+    <cfRule type="top10" dxfId="213" priority="739" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV8:AV71">
-    <cfRule type="top10" dxfId="262" priority="738" rank="2"/>
+    <cfRule type="top10" dxfId="212" priority="741" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW8:AW71">
-    <cfRule type="top10" dxfId="261" priority="740" rank="2"/>
+    <cfRule type="top10" dxfId="211" priority="743" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX8:AX71">
-    <cfRule type="top10" dxfId="260" priority="742" rank="2"/>
+    <cfRule type="top10" dxfId="210" priority="745" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY8:AY71">
-    <cfRule type="top10" dxfId="259" priority="744" rank="2"/>
+    <cfRule type="top10" dxfId="209" priority="747" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ8:AZ71">
-    <cfRule type="top10" dxfId="258" priority="746" rank="2"/>
+    <cfRule type="top10" dxfId="208" priority="749" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA8:BA71">
-    <cfRule type="top10" dxfId="257" priority="748" rank="2"/>
+    <cfRule type="top10" dxfId="207" priority="751" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB8:BB71">
-    <cfRule type="top10" dxfId="256" priority="750" rank="2"/>
+    <cfRule type="top10" dxfId="206" priority="753" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC8:BC71">
-    <cfRule type="top10" dxfId="255" priority="752" rank="2"/>
+    <cfRule type="top10" dxfId="205" priority="755" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD8:BD71">
-    <cfRule type="top10" dxfId="254" priority="754" rank="2"/>
+    <cfRule type="top10" dxfId="204" priority="757" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE8:BE71">
-    <cfRule type="top10" dxfId="253" priority="756" rank="2"/>
+    <cfRule type="top10" dxfId="203" priority="759" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF8:BF71">
-    <cfRule type="top10" dxfId="252" priority="758" rank="2"/>
+    <cfRule type="top10" dxfId="202" priority="761" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG8:BG71">
-    <cfRule type="top10" dxfId="251" priority="760" rank="2"/>
+    <cfRule type="top10" dxfId="201" priority="763" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH8:BH71">
-    <cfRule type="top10" dxfId="250" priority="762" rank="2"/>
+    <cfRule type="top10" dxfId="200" priority="765" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI8:BI71">
-    <cfRule type="top10" dxfId="249" priority="764" rank="2"/>
+    <cfRule type="top10" dxfId="199" priority="767" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -12459,6 +13271,267 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:P9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>779</v>
+      </c>
+      <c r="C4">
+        <v>3510.29</v>
+      </c>
+      <c r="D4">
+        <v>408.71</v>
+      </c>
+      <c r="E4">
+        <v>90.22</v>
+      </c>
+      <c r="F4">
+        <v>57.34</v>
+      </c>
+      <c r="G4">
+        <v>293.45999999999998</v>
+      </c>
+      <c r="H4">
+        <v>280.89</v>
+      </c>
+      <c r="I4">
+        <v>186.74</v>
+      </c>
+      <c r="J4">
+        <v>224.17</v>
+      </c>
+      <c r="K4">
+        <v>103.63</v>
+      </c>
+      <c r="L4">
+        <v>548.5</v>
+      </c>
+      <c r="M4">
+        <v>452.66</v>
+      </c>
+      <c r="N4">
+        <v>573.70000000000005</v>
+      </c>
+      <c r="O4">
+        <v>374.66</v>
+      </c>
+      <c r="P4">
+        <v>471.88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>780</v>
+      </c>
+      <c r="C5">
+        <v>3509.06</v>
+      </c>
+      <c r="D5">
+        <v>409.94</v>
+      </c>
+      <c r="E5">
+        <v>90.16</v>
+      </c>
+      <c r="F5">
+        <v>57.09</v>
+      </c>
+      <c r="G5">
+        <v>292.85000000000002</v>
+      </c>
+      <c r="H5">
+        <v>280.13</v>
+      </c>
+      <c r="I5">
+        <v>185.73</v>
+      </c>
+      <c r="J5">
+        <v>223.86</v>
+      </c>
+      <c r="K5">
+        <v>104.09</v>
+      </c>
+      <c r="L5">
+        <v>548.69000000000005</v>
+      </c>
+      <c r="M5">
+        <v>452.46</v>
+      </c>
+      <c r="N5">
+        <v>576.22</v>
+      </c>
+      <c r="O5">
+        <v>374.94</v>
+      </c>
+      <c r="P5">
+        <v>470.11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>780</v>
+      </c>
+      <c r="C6">
+        <v>3510.14</v>
+      </c>
+      <c r="D6">
+        <v>408.86</v>
+      </c>
+      <c r="E6">
+        <v>90.16</v>
+      </c>
+      <c r="F6">
+        <v>56.99</v>
+      </c>
+      <c r="G6">
+        <v>292.74</v>
+      </c>
+      <c r="H6">
+        <v>280.39</v>
+      </c>
+      <c r="I6">
+        <v>186.35</v>
+      </c>
+      <c r="J6">
+        <v>223.29</v>
+      </c>
+      <c r="K6">
+        <v>103.51</v>
+      </c>
+      <c r="L6">
+        <v>551.96</v>
+      </c>
+      <c r="M6">
+        <v>450.71</v>
+      </c>
+      <c r="N6">
+        <v>573.07000000000005</v>
+      </c>
+      <c r="O6">
+        <v>376.19</v>
+      </c>
+      <c r="P6">
+        <v>471.92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>779</v>
+      </c>
+      <c r="C7">
+        <v>3508.01</v>
+      </c>
+      <c r="D7">
+        <v>410.99</v>
+      </c>
+      <c r="E7">
+        <v>90.12</v>
+      </c>
+      <c r="F7">
+        <v>56.82</v>
+      </c>
+      <c r="G7">
+        <v>291.79000000000002</v>
+      </c>
+      <c r="H7">
+        <v>280.52999999999997</v>
+      </c>
+      <c r="I7">
+        <v>184.94</v>
+      </c>
+      <c r="J7">
+        <v>223.96</v>
+      </c>
+      <c r="K7">
+        <v>103.89</v>
+      </c>
+      <c r="L7">
+        <v>550.16</v>
+      </c>
+      <c r="M7">
+        <v>452.54</v>
+      </c>
+      <c r="N7">
+        <v>572.34</v>
+      </c>
+      <c r="O7">
+        <v>377.96</v>
+      </c>
+      <c r="P7">
+        <v>469.89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>AVERAGE(C4:C7)</f>
+        <v>3509.375</v>
+      </c>
+      <c r="D9" s="25">
+        <f t="shared" ref="D9:P9" si="0">AVERAGE(D4:D7)</f>
+        <v>409.625</v>
+      </c>
+      <c r="E9" s="25">
+        <f t="shared" si="0"/>
+        <v>90.164999999999992</v>
+      </c>
+      <c r="F9" s="25">
+        <f t="shared" si="0"/>
+        <v>57.06</v>
+      </c>
+      <c r="G9" s="25">
+        <f t="shared" si="0"/>
+        <v>292.70999999999998</v>
+      </c>
+      <c r="H9" s="25">
+        <f t="shared" si="0"/>
+        <v>280.48500000000001</v>
+      </c>
+      <c r="I9" s="25">
+        <f t="shared" si="0"/>
+        <v>185.94</v>
+      </c>
+      <c r="J9" s="25">
+        <f t="shared" si="0"/>
+        <v>223.82</v>
+      </c>
+      <c r="K9" s="25">
+        <f t="shared" si="0"/>
+        <v>103.78</v>
+      </c>
+      <c r="L9" s="25">
+        <f t="shared" si="0"/>
+        <v>549.82749999999999</v>
+      </c>
+      <c r="M9" s="25">
+        <f t="shared" si="0"/>
+        <v>452.09249999999997</v>
+      </c>
+      <c r="N9" s="25">
+        <f t="shared" si="0"/>
+        <v>573.8325000000001</v>
+      </c>
+      <c r="O9" s="25">
+        <f t="shared" si="0"/>
+        <v>375.9375</v>
+      </c>
+      <c r="P9" s="25">
+        <f t="shared" si="0"/>
+        <v>470.95000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA85"/>
   <sheetViews>
@@ -29450,332 +30523,332 @@
     <cfRule type="top10" priority="181" rank="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86:M93">
-    <cfRule type="top10" dxfId="248" priority="180" rank="2"/>
+    <cfRule type="top10" dxfId="448" priority="180" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N86:P93">
-    <cfRule type="top10" dxfId="247" priority="179" rank="2"/>
+    <cfRule type="top10" dxfId="447" priority="179" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q86:S93">
-    <cfRule type="top10" dxfId="246" priority="178" rank="2"/>
+    <cfRule type="top10" dxfId="446" priority="178" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T86:V93">
-    <cfRule type="top10" dxfId="245" priority="177" rank="2"/>
+    <cfRule type="top10" dxfId="445" priority="177" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W86:X93">
-    <cfRule type="top10" dxfId="244" priority="176" rank="2"/>
+    <cfRule type="top10" dxfId="444" priority="176" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y86:Z93">
-    <cfRule type="top10" dxfId="243" priority="175" rank="2"/>
+    <cfRule type="top10" dxfId="443" priority="175" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA86:AC93">
-    <cfRule type="top10" dxfId="242" priority="174" rank="2"/>
+    <cfRule type="top10" dxfId="442" priority="174" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD86:AE93">
-    <cfRule type="top10" dxfId="241" priority="173" rank="2"/>
+    <cfRule type="top10" dxfId="441" priority="173" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF86:AG93">
-    <cfRule type="top10" dxfId="240" priority="172" rank="2"/>
+    <cfRule type="top10" dxfId="440" priority="172" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN86:AN93">
-    <cfRule type="top10" dxfId="239" priority="171" rank="2"/>
+    <cfRule type="top10" dxfId="439" priority="171" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM86:AM93">
-    <cfRule type="top10" dxfId="238" priority="170" rank="2"/>
+    <cfRule type="top10" dxfId="438" priority="170" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50:M50 J8:M47">
-    <cfRule type="top10" dxfId="237" priority="431" rank="2"/>
+    <cfRule type="top10" dxfId="437" priority="431" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N50:P50 N8:P47">
-    <cfRule type="top10" dxfId="236" priority="433" rank="2"/>
+    <cfRule type="top10" dxfId="436" priority="433" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q50:S50 Q8:S47">
-    <cfRule type="top10" dxfId="235" priority="435" rank="2"/>
+    <cfRule type="top10" dxfId="435" priority="435" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA50:AC50 AA8:AC47">
-    <cfRule type="top10" dxfId="234" priority="437" rank="2"/>
+    <cfRule type="top10" dxfId="434" priority="437" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD50:AE50 AD8:AE47">
-    <cfRule type="top10" dxfId="233" priority="439" rank="2"/>
+    <cfRule type="top10" dxfId="433" priority="439" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF50:AG50 AF8:AG47">
-    <cfRule type="top10" dxfId="232" priority="441" rank="2"/>
+    <cfRule type="top10" dxfId="432" priority="441" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T50:V50 T8:V47">
-    <cfRule type="top10" dxfId="231" priority="445" rank="2"/>
+    <cfRule type="top10" dxfId="431" priority="445" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W50:X50 W8:X47">
-    <cfRule type="top10" dxfId="230" priority="447" rank="2"/>
+    <cfRule type="top10" dxfId="430" priority="447" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y50:Z50 Y8:Z47">
-    <cfRule type="top10" dxfId="229" priority="449" rank="2"/>
+    <cfRule type="top10" dxfId="429" priority="449" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO47:BX47 AN8:AN18 AN30:AN50">
-    <cfRule type="top10" dxfId="228" priority="451" rank="2"/>
+    <cfRule type="top10" dxfId="428" priority="451" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO48:AO50 AO8:AO18 AO30:AO46">
-    <cfRule type="top10" dxfId="227" priority="453" rank="2"/>
+    <cfRule type="top10" dxfId="427" priority="453" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP48:AP50 AP8:AP18 AP30:AP46">
-    <cfRule type="top10" dxfId="226" priority="455" rank="2"/>
+    <cfRule type="top10" dxfId="426" priority="455" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ48:AQ50 AQ8:AQ18 AQ30:AQ46">
-    <cfRule type="top10" dxfId="225" priority="457" rank="2"/>
+    <cfRule type="top10" dxfId="425" priority="457" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR48:AR50 AR8:AR18 AR30:AR46">
-    <cfRule type="top10" dxfId="224" priority="459" rank="2"/>
+    <cfRule type="top10" dxfId="424" priority="459" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS48:AS50 AS8:AS18 AS30:AS46">
-    <cfRule type="top10" dxfId="223" priority="461" rank="2"/>
+    <cfRule type="top10" dxfId="423" priority="461" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT48:AT50 AT8:AT18 AT30:AT46">
-    <cfRule type="top10" dxfId="222" priority="463" rank="2"/>
+    <cfRule type="top10" dxfId="422" priority="463" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU48:AU50 AU8:AU18 AU30:AU46">
-    <cfRule type="top10" dxfId="221" priority="465" rank="2"/>
+    <cfRule type="top10" dxfId="421" priority="465" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV48:AV50 AV8:AV18 AV30:AV46">
-    <cfRule type="top10" dxfId="220" priority="467" rank="2"/>
+    <cfRule type="top10" dxfId="420" priority="467" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW48:AW50 AW8:AW18 AW30:AW46">
-    <cfRule type="top10" dxfId="219" priority="469" rank="2"/>
+    <cfRule type="top10" dxfId="419" priority="469" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX48:AX50 AX8:AX18 AX30:AX46">
-    <cfRule type="top10" dxfId="218" priority="471" rank="2"/>
+    <cfRule type="top10" dxfId="418" priority="471" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY48:AY50 AY8:AY18 AY30:AY46">
-    <cfRule type="top10" dxfId="217" priority="473" rank="2"/>
+    <cfRule type="top10" dxfId="417" priority="473" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ48:AZ50 AZ8:AZ18 AZ30:AZ46">
-    <cfRule type="top10" dxfId="216" priority="475" rank="2"/>
+    <cfRule type="top10" dxfId="416" priority="475" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA48:BA50 BA8:BA18 BA30:BA46">
-    <cfRule type="top10" dxfId="215" priority="477" rank="2"/>
+    <cfRule type="top10" dxfId="415" priority="477" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB48:BB50 BB8:BB18 BB30:BB46">
-    <cfRule type="top10" dxfId="214" priority="479" rank="2"/>
+    <cfRule type="top10" dxfId="414" priority="479" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC48:BC50 BC8:BC18 BC30:BC46">
-    <cfRule type="top10" dxfId="213" priority="481" rank="2"/>
+    <cfRule type="top10" dxfId="413" priority="481" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD48:BD50 BD8:BD18 BD30:BD46">
-    <cfRule type="top10" dxfId="212" priority="483" rank="2"/>
+    <cfRule type="top10" dxfId="412" priority="483" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE48:BE50 BE8:BE18 BE30:BE46">
-    <cfRule type="top10" dxfId="211" priority="485" rank="2"/>
+    <cfRule type="top10" dxfId="411" priority="485" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF48:BF50 BF8:BF18 BF30:BF46">
-    <cfRule type="top10" dxfId="210" priority="487" rank="2"/>
+    <cfRule type="top10" dxfId="410" priority="487" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG48:BG50 BG8:BG18 BG30:BG46">
-    <cfRule type="top10" dxfId="209" priority="489" rank="2"/>
+    <cfRule type="top10" dxfId="409" priority="489" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH48:BH50 BH8:BH18 BH30:BH46">
-    <cfRule type="top10" dxfId="208" priority="491" rank="2"/>
+    <cfRule type="top10" dxfId="408" priority="491" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI48:BI50 BI8:BI18 BI30:BI46">
-    <cfRule type="top10" dxfId="207" priority="493" rank="2"/>
+    <cfRule type="top10" dxfId="407" priority="493" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ48:BJ50 BJ8:BJ18 BJ30:BJ46">
-    <cfRule type="top10" dxfId="206" priority="495" rank="2"/>
+    <cfRule type="top10" dxfId="406" priority="495" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK48:BK50 BK8:BK18 BK30:BK46">
-    <cfRule type="top10" dxfId="205" priority="497" rank="2"/>
+    <cfRule type="top10" dxfId="405" priority="497" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL48:BL50 BL8:BL18 BL30:BL46">
-    <cfRule type="top10" dxfId="204" priority="499" rank="2"/>
+    <cfRule type="top10" dxfId="404" priority="499" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM48:BM50 BM8:BM18 BM30:BM46">
-    <cfRule type="top10" dxfId="203" priority="501" rank="2"/>
+    <cfRule type="top10" dxfId="403" priority="501" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN48:BN50 BN8:BN18 BN30:BN46">
-    <cfRule type="top10" dxfId="202" priority="503" rank="2"/>
+    <cfRule type="top10" dxfId="402" priority="503" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO48:BO50 BO8:BO18 BO30:BO46">
-    <cfRule type="top10" dxfId="201" priority="505" rank="2"/>
+    <cfRule type="top10" dxfId="401" priority="505" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP48:BP50 BP8:BP18 BP30:BP46">
-    <cfRule type="top10" dxfId="200" priority="507" rank="2"/>
+    <cfRule type="top10" dxfId="400" priority="507" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ48:BQ50 BQ8:BQ18 BQ30:BQ46">
-    <cfRule type="top10" dxfId="199" priority="509" rank="2"/>
+    <cfRule type="top10" dxfId="399" priority="509" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR48:BR50 BR8:BR18 BR30:BR46">
-    <cfRule type="top10" dxfId="198" priority="511" rank="2"/>
+    <cfRule type="top10" dxfId="398" priority="511" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS48:BS50 BS8:BS18 BS30:BS46">
-    <cfRule type="top10" dxfId="197" priority="513" rank="2"/>
+    <cfRule type="top10" dxfId="397" priority="513" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT48:BT50 BT8:BT18 BT30:BT46">
-    <cfRule type="top10" dxfId="196" priority="515" rank="2"/>
+    <cfRule type="top10" dxfId="396" priority="515" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU48:BU50 BU8:BU18 BU30:BU46">
-    <cfRule type="top10" dxfId="195" priority="517" rank="2"/>
+    <cfRule type="top10" dxfId="395" priority="517" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV48:BV50 BV8:BV18 BV30:BV46">
-    <cfRule type="top10" dxfId="194" priority="519" rank="2"/>
+    <cfRule type="top10" dxfId="394" priority="519" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BW48:BW50 BW8:BW18 BW30:BW46">
-    <cfRule type="top10" dxfId="193" priority="521" rank="2"/>
+    <cfRule type="top10" dxfId="393" priority="521" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX48:BX50 BX8:BX18 BX30:BX46">
-    <cfRule type="top10" dxfId="192" priority="523" rank="2"/>
+    <cfRule type="top10" dxfId="392" priority="523" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ18 AJ30:AJ50">
-    <cfRule type="top10" dxfId="191" priority="815" rank="2"/>
+    <cfRule type="top10" dxfId="391" priority="815" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ19:AJ29">
-    <cfRule type="top10" dxfId="190" priority="1" rank="2"/>
+    <cfRule type="top10" dxfId="390" priority="1" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN19:AN29">
-    <cfRule type="top10" dxfId="189" priority="2" rank="2"/>
+    <cfRule type="top10" dxfId="389" priority="2" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO19:AO29">
-    <cfRule type="top10" dxfId="188" priority="3" rank="2"/>
+    <cfRule type="top10" dxfId="388" priority="3" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP19:AP29">
-    <cfRule type="top10" dxfId="187" priority="4" rank="2"/>
+    <cfRule type="top10" dxfId="387" priority="4" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ19:AQ29">
-    <cfRule type="top10" dxfId="186" priority="5" rank="2"/>
+    <cfRule type="top10" dxfId="386" priority="5" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR19:AR29">
-    <cfRule type="top10" dxfId="185" priority="6" rank="2"/>
+    <cfRule type="top10" dxfId="385" priority="6" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS19:AS29">
-    <cfRule type="top10" dxfId="184" priority="7" rank="2"/>
+    <cfRule type="top10" dxfId="384" priority="7" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT19:AT29">
-    <cfRule type="top10" dxfId="183" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="383" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU19:AU29">
-    <cfRule type="top10" dxfId="182" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="382" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV19:AV29">
-    <cfRule type="top10" dxfId="181" priority="10" rank="2"/>
+    <cfRule type="top10" dxfId="381" priority="10" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW19:AW29">
-    <cfRule type="top10" dxfId="180" priority="11" rank="2"/>
+    <cfRule type="top10" dxfId="380" priority="11" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX19:AX29">
-    <cfRule type="top10" dxfId="179" priority="12" rank="2"/>
+    <cfRule type="top10" dxfId="379" priority="12" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY19:AY29">
-    <cfRule type="top10" dxfId="178" priority="13" rank="2"/>
+    <cfRule type="top10" dxfId="378" priority="13" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ19:AZ29">
-    <cfRule type="top10" dxfId="177" priority="14" rank="2"/>
+    <cfRule type="top10" dxfId="377" priority="14" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA19:BA29">
-    <cfRule type="top10" dxfId="176" priority="15" rank="2"/>
+    <cfRule type="top10" dxfId="376" priority="15" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB19:BB29">
-    <cfRule type="top10" dxfId="175" priority="16" rank="2"/>
+    <cfRule type="top10" dxfId="375" priority="16" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC19:BC29">
-    <cfRule type="top10" dxfId="174" priority="17" rank="2"/>
+    <cfRule type="top10" dxfId="374" priority="17" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD19:BD29">
-    <cfRule type="top10" dxfId="173" priority="18" rank="2"/>
+    <cfRule type="top10" dxfId="373" priority="18" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE19:BE29">
-    <cfRule type="top10" dxfId="172" priority="19" rank="2"/>
+    <cfRule type="top10" dxfId="372" priority="19" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF19:BF29">
-    <cfRule type="top10" dxfId="171" priority="20" rank="2"/>
+    <cfRule type="top10" dxfId="371" priority="20" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG19:BG29">
-    <cfRule type="top10" dxfId="170" priority="21" rank="2"/>
+    <cfRule type="top10" dxfId="370" priority="21" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH19:BH29">
-    <cfRule type="top10" dxfId="169" priority="22" rank="2"/>
+    <cfRule type="top10" dxfId="369" priority="22" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI19:BI29">
-    <cfRule type="top10" dxfId="168" priority="23" rank="2"/>
+    <cfRule type="top10" dxfId="368" priority="23" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ19:BJ29">
-    <cfRule type="top10" dxfId="167" priority="24" rank="2"/>
+    <cfRule type="top10" dxfId="367" priority="24" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BK19:BK29">
-    <cfRule type="top10" dxfId="166" priority="25" rank="2"/>
+    <cfRule type="top10" dxfId="366" priority="25" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL19:BL29">
-    <cfRule type="top10" dxfId="165" priority="26" rank="2"/>
+    <cfRule type="top10" dxfId="365" priority="26" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM19:BM29">
-    <cfRule type="top10" dxfId="164" priority="27" rank="2"/>
+    <cfRule type="top10" dxfId="364" priority="27" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN19:BN29">
-    <cfRule type="top10" dxfId="163" priority="28" rank="2"/>
+    <cfRule type="top10" dxfId="363" priority="28" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO19:BO29">
-    <cfRule type="top10" dxfId="162" priority="29" rank="2"/>
+    <cfRule type="top10" dxfId="362" priority="29" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP19:BP29">
-    <cfRule type="top10" dxfId="161" priority="30" rank="2"/>
+    <cfRule type="top10" dxfId="361" priority="30" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ19:BQ29">
-    <cfRule type="top10" dxfId="160" priority="31" rank="2"/>
+    <cfRule type="top10" dxfId="360" priority="31" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR19:BR29">
-    <cfRule type="top10" dxfId="159" priority="32" rank="2"/>
+    <cfRule type="top10" dxfId="359" priority="32" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS19:BS29">
-    <cfRule type="top10" dxfId="158" priority="33" rank="2"/>
+    <cfRule type="top10" dxfId="358" priority="33" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BT19:BT29">
-    <cfRule type="top10" dxfId="157" priority="34" rank="2"/>
+    <cfRule type="top10" dxfId="357" priority="34" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU19:BU29">
-    <cfRule type="top10" dxfId="156" priority="35" rank="2"/>
+    <cfRule type="top10" dxfId="356" priority="35" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV19:BV29">
-    <cfRule type="top10" dxfId="155" priority="36" rank="2"/>
+    <cfRule type="top10" dxfId="355" priority="36" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BW19:BW29">
-    <cfRule type="top10" dxfId="154" priority="37" rank="2"/>
+    <cfRule type="top10" dxfId="354" priority="37" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX19:BX29">
-    <cfRule type="top10" dxfId="153" priority="38" rank="2"/>
+    <cfRule type="top10" dxfId="353" priority="38" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:M85">
-    <cfRule type="top10" dxfId="152" priority="816" rank="2"/>
+    <cfRule type="top10" dxfId="352" priority="816" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N51:P85">
-    <cfRule type="top10" dxfId="151" priority="818" rank="2"/>
+    <cfRule type="top10" dxfId="351" priority="818" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q51:S85">
-    <cfRule type="top10" dxfId="150" priority="820" rank="2"/>
+    <cfRule type="top10" dxfId="350" priority="820" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA51:AC85">
-    <cfRule type="top10" dxfId="149" priority="822" rank="2"/>
+    <cfRule type="top10" dxfId="349" priority="822" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD51:AE85">
-    <cfRule type="top10" dxfId="148" priority="824" rank="2"/>
+    <cfRule type="top10" dxfId="348" priority="824" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF51:AG85">
-    <cfRule type="top10" dxfId="147" priority="826" rank="2"/>
+    <cfRule type="top10" dxfId="347" priority="826" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ51:AJ85">
-    <cfRule type="top10" dxfId="146" priority="828" rank="2"/>
+    <cfRule type="top10" dxfId="346" priority="828" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T51:V85">
-    <cfRule type="top10" dxfId="145" priority="830" rank="2"/>
+    <cfRule type="top10" dxfId="345" priority="830" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W51:X85">
-    <cfRule type="top10" dxfId="144" priority="832" rank="2"/>
+    <cfRule type="top10" dxfId="344" priority="832" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y51:Z85">
-    <cfRule type="top10" dxfId="143" priority="834" rank="2"/>
+    <cfRule type="top10" dxfId="343" priority="834" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN51:BX85">
-    <cfRule type="top10" dxfId="142" priority="836" rank="2"/>
+    <cfRule type="top10" dxfId="342" priority="836" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI41"/>
   <sheetViews>
@@ -36784,154 +37857,154 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J8:J41">
-    <cfRule type="top10" dxfId="141" priority="48" rank="2"/>
+    <cfRule type="top10" dxfId="341" priority="48" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:K41">
-    <cfRule type="top10" dxfId="140" priority="47" rank="2"/>
+    <cfRule type="top10" dxfId="340" priority="47" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L41">
-    <cfRule type="top10" dxfId="139" priority="46" rank="2"/>
+    <cfRule type="top10" dxfId="339" priority="46" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:M41">
-    <cfRule type="top10" dxfId="138" priority="45" rank="2"/>
+    <cfRule type="top10" dxfId="338" priority="45" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C33 N8:N41">
-    <cfRule type="top10" dxfId="137" priority="44" rank="2"/>
+    <cfRule type="top10" dxfId="337" priority="44" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D33 O8:O41">
-    <cfRule type="top10" dxfId="136" priority="43" rank="2"/>
+    <cfRule type="top10" dxfId="336" priority="43" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:E33 P8:P41">
-    <cfRule type="top10" dxfId="135" priority="42" rank="2"/>
+    <cfRule type="top10" dxfId="335" priority="42" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:F33 Q8:Q41">
-    <cfRule type="top10" dxfId="134" priority="41" rank="2"/>
+    <cfRule type="top10" dxfId="334" priority="41" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G33 R8:R41">
-    <cfRule type="top10" dxfId="133" priority="40" rank="2"/>
+    <cfRule type="top10" dxfId="333" priority="40" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y8:Y41">
-    <cfRule type="top10" dxfId="132" priority="39" rank="2"/>
+    <cfRule type="top10" dxfId="332" priority="39" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X8:X41">
-    <cfRule type="top10" dxfId="131" priority="38" rank="2"/>
+    <cfRule type="top10" dxfId="331" priority="38" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z8:Z41">
-    <cfRule type="top10" dxfId="130" priority="37" rank="2"/>
+    <cfRule type="top10" dxfId="330" priority="37" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA8:AA41">
-    <cfRule type="top10" dxfId="129" priority="36" rank="2"/>
+    <cfRule type="top10" dxfId="329" priority="36" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB8:AB41">
-    <cfRule type="top10" dxfId="128" priority="35" rank="2"/>
+    <cfRule type="top10" dxfId="328" priority="35" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8:AC41">
-    <cfRule type="top10" dxfId="127" priority="34" rank="2"/>
+    <cfRule type="top10" dxfId="327" priority="34" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD8:AD41">
-    <cfRule type="top10" dxfId="126" priority="33" rank="2"/>
+    <cfRule type="top10" dxfId="326" priority="33" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AE41">
-    <cfRule type="top10" dxfId="125" priority="32" rank="2"/>
+    <cfRule type="top10" dxfId="325" priority="32" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF8:AF41">
-    <cfRule type="top10" dxfId="124" priority="31" rank="2"/>
+    <cfRule type="top10" dxfId="324" priority="31" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG8:AG41">
-    <cfRule type="top10" dxfId="123" priority="30" rank="2"/>
+    <cfRule type="top10" dxfId="323" priority="30" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH8:AH41">
-    <cfRule type="top10" dxfId="122" priority="29" rank="2"/>
+    <cfRule type="top10" dxfId="322" priority="29" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8:AI41">
-    <cfRule type="top10" dxfId="121" priority="28" rank="2"/>
+    <cfRule type="top10" dxfId="321" priority="28" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8:AJ41">
-    <cfRule type="top10" dxfId="120" priority="27" rank="2"/>
+    <cfRule type="top10" dxfId="320" priority="27" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8:AK41">
-    <cfRule type="top10" dxfId="119" priority="26" rank="2"/>
+    <cfRule type="top10" dxfId="319" priority="26" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL8:AL41">
-    <cfRule type="top10" dxfId="118" priority="25" rank="2"/>
+    <cfRule type="top10" dxfId="318" priority="25" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM8:AM41">
-    <cfRule type="top10" dxfId="117" priority="24" rank="2"/>
+    <cfRule type="top10" dxfId="317" priority="24" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN8:AN41">
-    <cfRule type="top10" dxfId="116" priority="23" rank="2"/>
+    <cfRule type="top10" dxfId="316" priority="23" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO8:AO41">
-    <cfRule type="top10" dxfId="115" priority="22" rank="2"/>
+    <cfRule type="top10" dxfId="315" priority="22" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP8:AP41">
-    <cfRule type="top10" dxfId="114" priority="21" rank="2"/>
+    <cfRule type="top10" dxfId="314" priority="21" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ8:AQ41">
-    <cfRule type="top10" dxfId="113" priority="20" rank="2"/>
+    <cfRule type="top10" dxfId="313" priority="20" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR8:AR41">
-    <cfRule type="top10" dxfId="112" priority="19" rank="2"/>
+    <cfRule type="top10" dxfId="312" priority="19" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS8:AS41">
-    <cfRule type="top10" dxfId="111" priority="18" rank="2"/>
+    <cfRule type="top10" dxfId="311" priority="18" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT8:AT41">
-    <cfRule type="top10" dxfId="110" priority="17" rank="2"/>
+    <cfRule type="top10" dxfId="310" priority="17" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU8:AU41">
-    <cfRule type="top10" dxfId="109" priority="16" rank="2"/>
+    <cfRule type="top10" dxfId="309" priority="16" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV8:AV41">
-    <cfRule type="top10" dxfId="108" priority="15" rank="2"/>
+    <cfRule type="top10" dxfId="308" priority="15" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW8:AW41">
-    <cfRule type="top10" dxfId="107" priority="14" rank="2"/>
+    <cfRule type="top10" dxfId="307" priority="14" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX8:AX41">
-    <cfRule type="top10" dxfId="106" priority="13" rank="2"/>
+    <cfRule type="top10" dxfId="306" priority="13" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY8:AY41">
-    <cfRule type="top10" dxfId="105" priority="12" rank="2"/>
+    <cfRule type="top10" dxfId="305" priority="12" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ8:AZ41">
-    <cfRule type="top10" dxfId="104" priority="11" rank="2"/>
+    <cfRule type="top10" dxfId="304" priority="11" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA8:BA41">
-    <cfRule type="top10" dxfId="103" priority="10" rank="2"/>
+    <cfRule type="top10" dxfId="303" priority="10" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB8:BB41">
-    <cfRule type="top10" dxfId="102" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="302" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC8:BC41">
-    <cfRule type="top10" dxfId="101" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="301" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD8:BD41">
-    <cfRule type="top10" dxfId="100" priority="7" rank="2"/>
+    <cfRule type="top10" dxfId="300" priority="7" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE8:BE41">
-    <cfRule type="top10" dxfId="99" priority="6" rank="2"/>
+    <cfRule type="top10" dxfId="299" priority="6" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF8:BF41">
-    <cfRule type="top10" dxfId="98" priority="5" rank="2"/>
+    <cfRule type="top10" dxfId="298" priority="5" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BG8:BG41">
-    <cfRule type="top10" dxfId="97" priority="4" rank="2"/>
+    <cfRule type="top10" dxfId="297" priority="4" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BH8:BH41">
-    <cfRule type="top10" dxfId="96" priority="3" rank="2"/>
+    <cfRule type="top10" dxfId="296" priority="3" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI8:BI41">
-    <cfRule type="top10" dxfId="95" priority="2" rank="2"/>
+    <cfRule type="top10" dxfId="295" priority="2" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U8:U41">
-    <cfRule type="top10" dxfId="94" priority="1" rank="2"/>
+    <cfRule type="top10" dxfId="294" priority="1" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AC42"/>
   <sheetViews>

</xml_diff>